<commit_message>
a new row added
</commit_message>
<xml_diff>
--- a/Programming-Basics-Book-Project-Plan.xlsx
+++ b/Programming-Basics-Book-Project-Plan.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAKOV\Programming-Basics-Book\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="306"/>
   </bookViews>
   <sheets>
     <sheet name="Programming Basics Book - Plan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Име на глава</t>
   </si>
@@ -172,6 +167,9 @@
   </si>
   <si>
     <t>Само трябва да се преправи в стила на учебника. Да се обнови за C# 6 и VS 2015. Вместо Mono да се дадат по-адекватни примери за C# разработка под Linux.</t>
+  </si>
+  <si>
+    <t>Нов ред</t>
   </si>
 </sst>
 </file>
@@ -311,36 +309,36 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1668,13 +1666,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,31 +1689,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1724,7 +1722,7 @@
       <c r="G2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1741,7 +1739,7 @@
       <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -1764,7 +1762,7 @@
       <c r="D4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>0</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -1774,142 +1772,142 @@
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>0.8</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="18">
         <v>0.9</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <v>0.8</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <v>0.9</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <v>0.9</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <v>0.9</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
@@ -1925,7 +1923,7 @@
       <c r="D11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>0</v>
       </c>
       <c r="F11" s="8" t="s">
@@ -1948,7 +1946,7 @@
       <c r="D12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>0.2</v>
       </c>
       <c r="F12" s="9" t="s">
@@ -1971,7 +1969,7 @@
       <c r="D13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>0.2</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -1979,6 +1977,14 @@
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>